<commit_message>
temp tol changed to 5C
</commit_message>
<xml_diff>
--- a/test files/P552 MCA PV AUX LIMITS.xlsx
+++ b/test files/P552 MCA PV AUX LIMITS.xlsx
@@ -265,7 +265,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -301,11 +301,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -419,6 +432,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,7 +720,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,8 +1347,8 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
@@ -1341,34 +1357,34 @@
       <c r="B26" s="9">
         <v>9</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="2">
         <v>1.093</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="2">
         <v>1.335</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="2">
         <v>0.44500000000000001</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="2">
         <v>0.54400000000000004</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="2">
         <v>1.5049999999999999</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="2">
         <v>1.839</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="2">
         <v>2.8439999999999999</v>
       </c>
-      <c r="J26" s="7">
+      <c r="J26" s="2">
         <v>3.129</v>
       </c>
-      <c r="K26" s="7">
+      <c r="K26" s="2">
         <v>1.905</v>
       </c>
-      <c r="L26" s="7">
+      <c r="L26" s="2">
         <v>2.3290000000000002</v>
       </c>
     </row>
@@ -1561,11 +1577,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="A30:A32"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A18:A20"/>
@@ -1576,6 +1587,11 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="I12:J12"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A30:A32"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="F5:F7"/>
   </mergeCells>

</xml_diff>